<commit_message>
updated old models and added Tesla, ASML, Enphase
</commit_message>
<xml_diff>
--- a/Abbvie DCF 10-21-22.xlsx
+++ b/Abbvie DCF 10-21-22.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bina/Documents/financial-modeling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DF01A9DD-13ED-9643-BFF8-888E5A755F44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC5C9A6F-2E86-6D47-89EC-E237FC814A9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23800" yWindow="460" windowWidth="27400" windowHeight="26980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2160" yWindow="460" windowWidth="26480" windowHeight="26980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -380,9 +380,6 @@
     <t>Revenue Growth YoY %</t>
   </si>
   <si>
-    <t>5 Year Revenue CAGR</t>
-  </si>
-  <si>
     <t>Weight of Debt</t>
   </si>
   <si>
@@ -395,9 +392,6 @@
     <t>Market Cap (10/23)</t>
   </si>
   <si>
-    <t>5 Year FCF CAGR</t>
-  </si>
-  <si>
     <t>Terminal Value</t>
   </si>
   <si>
@@ -432,6 +426,12 @@
   </si>
   <si>
     <t>Upside / Downside</t>
+  </si>
+  <si>
+    <t>10 Year FCF CAGR</t>
+  </si>
+  <si>
+    <t>10 Year Revenue CAGR</t>
   </si>
 </sst>
 </file>
@@ -711,9 +711,6 @@
     <xf numFmtId="9" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -761,6 +758,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="10" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1079,10 +1079,10 @@
   <dimension ref="A1:U111"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="J66" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="N65" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="O120" sqref="O120"/>
+      <selection pane="bottomRight" activeCell="T67" sqref="T67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1093,7 +1093,7 @@
     <col min="15" max="15" width="13.5" customWidth="1"/>
     <col min="16" max="16" width="13" customWidth="1"/>
     <col min="17" max="17" width="16.83203125" customWidth="1"/>
-    <col min="18" max="18" width="22.33203125" style="20" customWidth="1"/>
+    <col min="18" max="18" width="28.1640625" style="20" customWidth="1"/>
     <col min="19" max="19" width="12.33203125" customWidth="1"/>
     <col min="20" max="20" width="11.5" customWidth="1"/>
     <col min="21" max="21" width="16.1640625" customWidth="1"/>
@@ -1139,7 +1139,7 @@
       <c r="M1" s="8">
         <v>2020</v>
       </c>
-      <c r="N1" s="44">
+      <c r="N1" s="43">
         <v>2021</v>
       </c>
       <c r="O1" s="33">
@@ -1149,7 +1149,7 @@
         <v>2023</v>
       </c>
       <c r="Q1" s="34" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="21" x14ac:dyDescent="0.25">
@@ -1192,7 +1192,7 @@
       <c r="M2" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="N2" s="45" t="s">
+      <c r="N2" s="44" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1236,11 +1236,11 @@
       <c r="M3" s="1">
         <v>45804000000</v>
       </c>
-      <c r="N3" s="46">
+      <c r="N3" s="45">
         <v>56197000000</v>
       </c>
-      <c r="R3" s="37" t="s">
-        <v>115</v>
+      <c r="R3" s="59" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:18" s="29" customFormat="1" ht="19" x14ac:dyDescent="0.25">
@@ -1295,13 +1295,13 @@
         <f t="shared" ref="M4" si="10">(M3/L3)-1</f>
         <v>0.37690134070823067</v>
       </c>
-      <c r="N4" s="47">
+      <c r="N4" s="46">
         <f t="shared" ref="N4" si="11">(N3/M3)-1</f>
         <v>0.22690158064797838</v>
       </c>
       <c r="R4" s="30">
-        <f>(N4+M4+L4+K4+J4)/5</f>
-        <v>0.17616295351005209</v>
+        <f>(N4+M4+L4+K4+J4+I4+H4+G4+F4+E4)/10</f>
+        <v>0.12858610172439888</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="19" x14ac:dyDescent="0.25">
@@ -1344,7 +1344,7 @@
       <c r="M5" s="1">
         <v>15387000000</v>
       </c>
-      <c r="N5" s="46">
+      <c r="N5" s="45">
         <v>17446000000</v>
       </c>
     </row>
@@ -1388,7 +1388,7 @@
       <c r="M6" s="10">
         <v>30417000000</v>
       </c>
-      <c r="N6" s="48">
+      <c r="N6" s="47">
         <v>38751000000</v>
       </c>
     </row>
@@ -1432,7 +1432,7 @@
       <c r="M7" s="2">
         <v>0.66410000000000002</v>
       </c>
-      <c r="N7" s="49">
+      <c r="N7" s="48">
         <v>0.68959999999999999</v>
       </c>
     </row>
@@ -1476,7 +1476,7 @@
       <c r="M8" s="1">
         <v>6557000000</v>
       </c>
-      <c r="N8" s="46">
+      <c r="N8" s="45">
         <v>7084000000</v>
       </c>
     </row>
@@ -1520,7 +1520,7 @@
       <c r="M9" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="N9" s="46" t="s">
+      <c r="N9" s="45" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1564,7 +1564,7 @@
       <c r="M10" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="N10" s="46" t="s">
+      <c r="N10" s="45" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1608,7 +1608,7 @@
       <c r="M11" s="1">
         <v>11299000000</v>
       </c>
-      <c r="N11" s="46">
+      <c r="N11" s="45">
         <v>12349000000</v>
       </c>
     </row>
@@ -1652,7 +1652,7 @@
       <c r="M12" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="N12" s="46">
+      <c r="N12" s="45">
         <v>432000000</v>
       </c>
     </row>
@@ -1696,7 +1696,7 @@
       <c r="M13" s="1">
         <v>17856000000</v>
       </c>
-      <c r="N13" s="46">
+      <c r="N13" s="45">
         <v>19865000000</v>
       </c>
     </row>
@@ -1740,7 +1740,7 @@
       <c r="M14" s="1">
         <v>33243000000</v>
       </c>
-      <c r="N14" s="46">
+      <c r="N14" s="45">
         <v>37311000000</v>
       </c>
     </row>
@@ -1784,7 +1784,7 @@
       <c r="M15" s="1">
         <v>2454000000</v>
       </c>
-      <c r="N15" s="46">
+      <c r="N15" s="45">
         <v>2423000000</v>
       </c>
     </row>
@@ -1828,7 +1828,7 @@
       <c r="M16" s="1">
         <v>6471000000</v>
       </c>
-      <c r="N16" s="46">
+      <c r="N16" s="45">
         <v>8521000000</v>
       </c>
     </row>
@@ -1872,7 +1872,7 @@
       <c r="M17" s="10">
         <v>12317000000</v>
       </c>
-      <c r="N17" s="48">
+      <c r="N17" s="47">
         <v>23926000000</v>
       </c>
     </row>
@@ -1916,7 +1916,7 @@
       <c r="M18" s="2">
         <v>0.26889999999999997</v>
       </c>
-      <c r="N18" s="49">
+      <c r="N18" s="48">
         <v>0.42580000000000001</v>
       </c>
     </row>
@@ -1960,7 +1960,7 @@
       <c r="M19" s="10">
         <v>11363000000</v>
       </c>
-      <c r="N19" s="48">
+      <c r="N19" s="47">
         <v>17924000000</v>
       </c>
     </row>
@@ -2004,7 +2004,7 @@
       <c r="M20" s="2">
         <v>0.24809999999999999</v>
       </c>
-      <c r="N20" s="49">
+      <c r="N20" s="48">
         <v>0.31890000000000002</v>
       </c>
     </row>
@@ -2048,7 +2048,7 @@
       <c r="M21" s="1">
         <v>-7965000000</v>
       </c>
-      <c r="N21" s="46">
+      <c r="N21" s="45">
         <v>-4935000000</v>
       </c>
     </row>
@@ -2092,7 +2092,7 @@
       <c r="M22" s="10">
         <v>3398000000</v>
       </c>
-      <c r="N22" s="48">
+      <c r="N22" s="47">
         <v>12989000000</v>
       </c>
     </row>
@@ -2136,7 +2136,7 @@
       <c r="M23" s="2">
         <v>7.4200000000000002E-2</v>
       </c>
-      <c r="N23" s="49">
+      <c r="N23" s="48">
         <v>0.2311</v>
       </c>
     </row>
@@ -2180,7 +2180,7 @@
       <c r="M24" s="1">
         <v>-1224000000</v>
       </c>
-      <c r="N24" s="46">
+      <c r="N24" s="45">
         <v>1440000000</v>
       </c>
     </row>
@@ -2224,7 +2224,7 @@
       <c r="M25" s="11">
         <v>4616000000</v>
       </c>
-      <c r="N25" s="50">
+      <c r="N25" s="49">
         <v>11542000000</v>
       </c>
     </row>
@@ -2268,7 +2268,7 @@
       <c r="M26" s="2">
         <v>0.1008</v>
       </c>
-      <c r="N26" s="49">
+      <c r="N26" s="48">
         <v>0.2054</v>
       </c>
     </row>
@@ -2312,7 +2312,7 @@
       <c r="M27" s="12">
         <v>2.62</v>
       </c>
-      <c r="N27" s="51">
+      <c r="N27" s="50">
         <v>6.53</v>
       </c>
     </row>
@@ -2356,7 +2356,7 @@
       <c r="M28" s="12">
         <v>2.62</v>
       </c>
-      <c r="N28" s="51">
+      <c r="N28" s="50">
         <v>6.45</v>
       </c>
     </row>
@@ -2400,7 +2400,7 @@
       <c r="M29" s="1">
         <v>1765132819</v>
       </c>
-      <c r="N29" s="46">
+      <c r="N29" s="45">
         <v>1768337696</v>
       </c>
     </row>
@@ -2444,7 +2444,7 @@
       <c r="M30" s="1">
         <v>1765132819</v>
       </c>
-      <c r="N30" s="46">
+      <c r="N30" s="45">
         <v>1777000000</v>
       </c>
     </row>
@@ -2488,11 +2488,11 @@
       <c r="M31" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="N31" s="52" t="s">
+      <c r="N31" s="51" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="40" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" ht="21" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>29</v>
       </c>
@@ -2532,7 +2532,7 @@
       <c r="M32" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="N32" s="45" t="s">
+      <c r="N32" s="44" t="s">
         <v>91</v>
       </c>
       <c r="R32" s="25" t="s">
@@ -2581,7 +2581,7 @@
       <c r="M33" s="1">
         <v>8449000000</v>
       </c>
-      <c r="N33" s="46">
+      <c r="N33" s="45">
         <v>9746000000</v>
       </c>
       <c r="R33" s="22" t="s">
@@ -2633,7 +2633,7 @@
       <c r="M34" s="1">
         <v>30000000</v>
       </c>
-      <c r="N34" s="46">
+      <c r="N34" s="45">
         <v>84000000</v>
       </c>
       <c r="R34" s="22" t="s">
@@ -2685,7 +2685,7 @@
       <c r="M35" s="1">
         <v>8479000000</v>
       </c>
-      <c r="N35" s="46">
+      <c r="N35" s="45">
         <v>9830000000</v>
       </c>
       <c r="R35" s="22" t="s">
@@ -2737,7 +2737,7 @@
       <c r="M36" s="1">
         <v>8822000000</v>
       </c>
-      <c r="N36" s="46">
+      <c r="N36" s="45">
         <v>9977000000</v>
       </c>
       <c r="R36" s="23" t="s">
@@ -2789,7 +2789,7 @@
       <c r="M37" s="1">
         <v>3310000000</v>
       </c>
-      <c r="N37" s="46">
+      <c r="N37" s="45">
         <v>3128000000</v>
       </c>
       <c r="R37" s="22" t="s">
@@ -2841,7 +2841,7 @@
       <c r="M38" s="1">
         <v>3562000000</v>
       </c>
-      <c r="N38" s="46">
+      <c r="N38" s="45">
         <v>4993000000</v>
       </c>
       <c r="R38" s="22" t="s">
@@ -2893,7 +2893,7 @@
       <c r="M39" s="10">
         <v>24173000000</v>
       </c>
-      <c r="N39" s="48">
+      <c r="N39" s="47">
         <v>27928000000</v>
       </c>
       <c r="R39" s="23" t="s">
@@ -2945,7 +2945,7 @@
       <c r="M40" s="1">
         <v>5248000000</v>
       </c>
-      <c r="N40" s="46">
+      <c r="N40" s="45">
         <v>5110000000</v>
       </c>
       <c r="R40" s="23" t="s">
@@ -2997,14 +2997,14 @@
       <c r="M41" s="1">
         <v>33124000000</v>
       </c>
-      <c r="N41" s="46">
+      <c r="N41" s="45">
         <v>32379000000</v>
       </c>
       <c r="R41" s="22"/>
       <c r="S41" s="15"/>
       <c r="T41" s="15"/>
     </row>
-    <row r="42" spans="1:20" ht="40" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" ht="20" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>39</v>
       </c>
@@ -3044,7 +3044,7 @@
       <c r="M42" s="1">
         <v>82876000000</v>
       </c>
-      <c r="N42" s="46">
+      <c r="N42" s="45">
         <v>75951000000</v>
       </c>
       <c r="R42" s="25" t="s">
@@ -3093,7 +3093,7 @@
       <c r="M43" s="1">
         <v>116000000000</v>
       </c>
-      <c r="N43" s="46">
+      <c r="N43" s="45">
         <v>108330000000</v>
       </c>
       <c r="R43" s="22" t="s">
@@ -3144,7 +3144,7 @@
       <c r="M44" s="1">
         <v>293000000</v>
       </c>
-      <c r="N44" s="46">
+      <c r="N44" s="45">
         <v>277000000</v>
       </c>
       <c r="R44" s="22" t="s">
@@ -3195,7 +3195,7 @@
       <c r="M45" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="N45" s="46" t="s">
+      <c r="N45" s="45" t="s">
         <v>92</v>
       </c>
       <c r="R45" s="22" t="s">
@@ -3246,7 +3246,7 @@
       <c r="M46" s="1">
         <v>4851000000</v>
       </c>
-      <c r="N46" s="46">
+      <c r="N46" s="45">
         <v>4884000000</v>
       </c>
       <c r="R46" s="23" t="s">
@@ -3298,14 +3298,14 @@
       <c r="M47" s="1">
         <v>126392000000</v>
       </c>
-      <c r="N47" s="46">
+      <c r="N47" s="45">
         <v>118601000000</v>
       </c>
       <c r="R47" s="22"/>
       <c r="S47" s="15"/>
       <c r="T47" s="15"/>
     </row>
-    <row r="48" spans="1:20" ht="40" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" ht="20" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>45</v>
       </c>
@@ -3345,14 +3345,14 @@
       <c r="M48" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="N48" s="46" t="s">
+      <c r="N48" s="45" t="s">
         <v>92</v>
       </c>
       <c r="R48" s="26" t="s">
         <v>109</v>
       </c>
       <c r="S48" s="24" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="T48" s="24" t="s">
         <v>113</v>
@@ -3398,7 +3398,7 @@
       <c r="M49" s="11">
         <v>150565000000</v>
       </c>
-      <c r="N49" s="50">
+      <c r="N49" s="49">
         <v>146529000000</v>
       </c>
       <c r="R49" s="22" t="s">
@@ -3413,7 +3413,7 @@
         <v>0.22776253103800598</v>
       </c>
       <c r="U49" s="31" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="50" spans="1:21" ht="21" thickTop="1" x14ac:dyDescent="0.25">
@@ -3456,11 +3456,11 @@
       <c r="M50" s="1">
         <v>2276000000</v>
       </c>
-      <c r="N50" s="46">
+      <c r="N50" s="45">
         <v>2882000000</v>
       </c>
       <c r="R50" s="22" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="S50" s="16">
         <v>260000000000</v>
@@ -3470,7 +3470,7 @@
         <v>0.77223746896199408</v>
       </c>
       <c r="U50" s="31" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="51" spans="1:21" ht="20" x14ac:dyDescent="0.25">
@@ -3513,7 +3513,7 @@
       <c r="M51" s="1">
         <v>8502000000</v>
       </c>
-      <c r="N51" s="46">
+      <c r="N51" s="45">
         <v>12495000000</v>
       </c>
       <c r="R51" s="22" t="s">
@@ -3565,7 +3565,7 @@
       <c r="M52" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="N52" s="46" t="s">
+      <c r="N52" s="45" t="s">
         <v>92</v>
       </c>
       <c r="R52" s="22"/>
@@ -3612,7 +3612,7 @@
       <c r="M53" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="N53" s="46" t="s">
+      <c r="N53" s="45" t="s">
         <v>92</v>
       </c>
       <c r="R53" s="21" t="s">
@@ -3661,7 +3661,7 @@
       <c r="M54" s="1">
         <v>17883000000</v>
       </c>
-      <c r="N54" s="46">
+      <c r="N54" s="45">
         <v>19817000000</v>
       </c>
       <c r="R54" s="23" t="s">
@@ -3713,7 +3713,7 @@
       <c r="M55" s="10">
         <v>28661000000</v>
       </c>
-      <c r="N55" s="48">
+      <c r="N55" s="47">
         <v>35194000000</v>
       </c>
     </row>
@@ -3757,7 +3757,7 @@
       <c r="M56" s="1">
         <v>77554000000</v>
       </c>
-      <c r="N56" s="46">
+      <c r="N56" s="45">
         <v>64189000000</v>
       </c>
     </row>
@@ -3801,7 +3801,7 @@
       <c r="M57" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="N57" s="46" t="s">
+      <c r="N57" s="45" t="s">
         <v>92</v>
       </c>
     </row>
@@ -3845,7 +3845,7 @@
       <c r="M58" s="1">
         <v>3646000000</v>
       </c>
-      <c r="N58" s="46">
+      <c r="N58" s="45">
         <v>3009000000</v>
       </c>
     </row>
@@ -3889,7 +3889,7 @@
       <c r="M59" s="1">
         <v>27607000000</v>
       </c>
-      <c r="N59" s="46">
+      <c r="N59" s="45">
         <v>28701000000</v>
       </c>
     </row>
@@ -3933,7 +3933,7 @@
       <c r="M60" s="1">
         <v>108807000000</v>
       </c>
-      <c r="N60" s="46">
+      <c r="N60" s="45">
         <v>95899000000</v>
       </c>
     </row>
@@ -3977,7 +3977,7 @@
       <c r="M61" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="N61" s="46" t="s">
+      <c r="N61" s="45" t="s">
         <v>92</v>
       </c>
     </row>
@@ -4021,7 +4021,7 @@
       <c r="M62" s="10">
         <v>137468000000</v>
       </c>
-      <c r="N62" s="48">
+      <c r="N62" s="47">
         <v>131093000000</v>
       </c>
     </row>
@@ -4065,7 +4065,7 @@
       <c r="M63" s="1">
         <v>18000000</v>
       </c>
-      <c r="N63" s="46">
+      <c r="N63" s="45">
         <v>18000000</v>
       </c>
     </row>
@@ -4109,7 +4109,7 @@
       <c r="M64" s="1">
         <v>1055000000</v>
       </c>
-      <c r="N64" s="46">
+      <c r="N64" s="45">
         <v>3127000000</v>
       </c>
     </row>
@@ -4153,7 +4153,7 @@
       <c r="M65" s="1">
         <v>-3117000000</v>
       </c>
-      <c r="N65" s="46">
+      <c r="N65" s="45">
         <v>-2899000000</v>
       </c>
     </row>
@@ -4197,7 +4197,7 @@
       <c r="M66" s="1">
         <v>15120000000</v>
       </c>
-      <c r="N66" s="46">
+      <c r="N66" s="45">
         <v>15162000000</v>
       </c>
     </row>
@@ -4241,7 +4241,7 @@
       <c r="M67" s="10">
         <v>13076000000</v>
       </c>
-      <c r="N67" s="48">
+      <c r="N67" s="47">
         <v>15408000000</v>
       </c>
     </row>
@@ -4285,7 +4285,7 @@
       <c r="M68" s="11">
         <v>150544000000</v>
       </c>
-      <c r="N68" s="50">
+      <c r="N68" s="49">
         <v>146501000000</v>
       </c>
     </row>
@@ -4329,7 +4329,7 @@
       <c r="M69" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="N69" s="52" t="s">
+      <c r="N69" s="51" t="s">
         <v>93</v>
       </c>
     </row>
@@ -4373,7 +4373,7 @@
       <c r="M70" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="N70" s="45" t="s">
+      <c r="N70" s="44" t="s">
         <v>91</v>
       </c>
     </row>
@@ -4417,7 +4417,7 @@
       <c r="M71" s="1">
         <v>4622000000</v>
       </c>
-      <c r="N71" s="46">
+      <c r="N71" s="45">
         <v>11549000000</v>
       </c>
     </row>
@@ -4461,7 +4461,7 @@
       <c r="M72" s="1">
         <v>6471000000</v>
       </c>
-      <c r="N72" s="46">
+      <c r="N72" s="45">
         <v>8521000000</v>
       </c>
     </row>
@@ -4505,7 +4505,7 @@
       <c r="M73" s="1">
         <v>-2325000000</v>
       </c>
-      <c r="N73" s="46">
+      <c r="N73" s="45">
         <v>-898000000</v>
       </c>
     </row>
@@ -4549,7 +4549,7 @@
       <c r="M74" s="1">
         <v>753000000</v>
       </c>
-      <c r="N74" s="46">
+      <c r="N74" s="45">
         <v>692000000</v>
       </c>
     </row>
@@ -4593,7 +4593,7 @@
       <c r="M75" s="1">
         <v>106000000</v>
       </c>
-      <c r="N75" s="46">
+      <c r="N75" s="45">
         <v>-1322000000</v>
       </c>
     </row>
@@ -4637,7 +4637,7 @@
       <c r="M76" s="1">
         <v>-929000000</v>
       </c>
-      <c r="N76" s="46">
+      <c r="N76" s="45">
         <v>-1321000000</v>
       </c>
     </row>
@@ -4681,7 +4681,7 @@
       <c r="M77" s="1">
         <v>-40000000</v>
       </c>
-      <c r="N77" s="46">
+      <c r="N77" s="45">
         <v>-142000000</v>
       </c>
     </row>
@@ -4725,7 +4725,7 @@
       <c r="M78" s="1">
         <v>1514000000</v>
       </c>
-      <c r="N78" s="46">
+      <c r="N78" s="45">
         <v>1628000000</v>
       </c>
     </row>
@@ -4769,7 +4769,7 @@
       <c r="M79" s="1">
         <v>-573000000</v>
       </c>
-      <c r="N79" s="46">
+      <c r="N79" s="45">
         <v>-1290000000</v>
       </c>
     </row>
@@ -4813,7 +4813,7 @@
       <c r="M80" s="1">
         <v>7961000000</v>
       </c>
-      <c r="N80" s="46">
+      <c r="N80" s="45">
         <v>4235000000</v>
       </c>
     </row>
@@ -4857,7 +4857,7 @@
       <c r="M81" s="10">
         <v>17588000000</v>
       </c>
-      <c r="N81" s="48">
+      <c r="N81" s="47">
         <v>22777000000</v>
       </c>
     </row>
@@ -4901,7 +4901,7 @@
       <c r="M82" s="1">
         <v>-798000000</v>
       </c>
-      <c r="N82" s="46">
+      <c r="N82" s="45">
         <v>-787000000</v>
       </c>
     </row>
@@ -4945,7 +4945,7 @@
       <c r="M83" s="1">
         <v>-39610000000</v>
       </c>
-      <c r="N83" s="46">
+      <c r="N83" s="45">
         <v>-1902000000</v>
       </c>
     </row>
@@ -4989,7 +4989,7 @@
       <c r="M84" s="1">
         <v>-61000000</v>
       </c>
-      <c r="N84" s="46">
+      <c r="N84" s="45">
         <v>-119000000</v>
       </c>
     </row>
@@ -5033,7 +5033,7 @@
       <c r="M85" s="1">
         <v>1525000000</v>
       </c>
-      <c r="N85" s="46">
+      <c r="N85" s="45">
         <v>98000000</v>
       </c>
     </row>
@@ -5077,7 +5077,7 @@
       <c r="M86" s="1">
         <v>1387000000</v>
       </c>
-      <c r="N86" s="46">
+      <c r="N86" s="45">
         <v>366000000</v>
       </c>
     </row>
@@ -5121,7 +5121,7 @@
       <c r="M87" s="10">
         <v>-37557000000</v>
       </c>
-      <c r="N87" s="48">
+      <c r="N87" s="47">
         <v>-2344000000</v>
       </c>
     </row>
@@ -5165,7 +5165,7 @@
       <c r="M88" s="1">
         <v>-5683000000</v>
       </c>
-      <c r="N88" s="46">
+      <c r="N88" s="45">
         <v>-9414000000</v>
       </c>
     </row>
@@ -5209,7 +5209,7 @@
       <c r="M89" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="N89" s="46" t="s">
+      <c r="N89" s="45" t="s">
         <v>92</v>
       </c>
     </row>
@@ -5253,7 +5253,7 @@
       <c r="M90" s="1">
         <v>-978000000</v>
       </c>
-      <c r="N90" s="46">
+      <c r="N90" s="45">
         <v>-934000000</v>
       </c>
     </row>
@@ -5297,7 +5297,7 @@
       <c r="M91" s="1">
         <v>-7716000000</v>
       </c>
-      <c r="N91" s="46">
+      <c r="N91" s="45">
         <v>-9261000000</v>
       </c>
     </row>
@@ -5341,7 +5341,7 @@
       <c r="M92" s="1">
         <v>2876000000</v>
       </c>
-      <c r="N92" s="46">
+      <c r="N92" s="45">
         <v>570000000</v>
       </c>
     </row>
@@ -5385,7 +5385,7 @@
       <c r="M93" s="10">
         <v>-11501000000</v>
       </c>
-      <c r="N93" s="48">
+      <c r="N93" s="47">
         <v>-19039000000</v>
       </c>
     </row>
@@ -5429,7 +5429,7 @@
       <c r="M94" s="1">
         <v>-5000000</v>
       </c>
-      <c r="N94" s="46">
+      <c r="N94" s="45">
         <v>-97000000</v>
       </c>
     </row>
@@ -5473,7 +5473,7 @@
       <c r="M95" s="10">
         <v>-31475000000</v>
       </c>
-      <c r="N95" s="48">
+      <c r="N95" s="47">
         <v>1297000000</v>
       </c>
     </row>
@@ -5517,7 +5517,7 @@
       <c r="M96" s="1">
         <v>39924000000</v>
       </c>
-      <c r="N96" s="46">
+      <c r="N96" s="45">
         <v>8449000000</v>
       </c>
     </row>
@@ -5561,16 +5561,16 @@
       <c r="M97" s="11">
         <v>8449000000</v>
       </c>
-      <c r="N97" s="50">
+      <c r="N97" s="49">
         <v>9746000000</v>
       </c>
-      <c r="O97" s="43">
+      <c r="O97" s="42">
         <v>1</v>
       </c>
-      <c r="P97" s="43">
+      <c r="P97" s="42">
         <v>2</v>
       </c>
-      <c r="Q97" s="42">
+      <c r="Q97" s="41">
         <v>2</v>
       </c>
     </row>
@@ -5614,124 +5614,124 @@
       <c r="M98" s="1">
         <v>16790000000</v>
       </c>
-      <c r="N98" s="46">
+      <c r="N98" s="45">
         <v>21990000000</v>
       </c>
-      <c r="O98" s="39">
+      <c r="O98" s="38">
         <f>N98*(1+O99)</f>
-        <v>28147200000</v>
-      </c>
-      <c r="P98" s="39">
+        <v>25948200000</v>
+      </c>
+      <c r="P98" s="38">
         <f>O98*(1+P99)</f>
-        <v>36028416000</v>
-      </c>
-      <c r="Q98" s="39">
+        <v>30618876000</v>
+      </c>
+      <c r="Q98" s="38">
         <f>(P98*(1+Q99))/(S54-Q99)</f>
-        <v>1016725611101.6926</v>
-      </c>
-      <c r="R98" s="38" t="s">
-        <v>120</v>
+        <v>864067835020.74988</v>
+      </c>
+      <c r="R98" s="37" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="99" spans="1:18" s="36" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A99" s="27" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B99" s="35" t="e">
-        <f>(B98/A98)-1</f>
+        <f t="shared" ref="B99:N99" si="12">(B98/A98)-1</f>
         <v>#VALUE!</v>
       </c>
       <c r="C99" s="35">
-        <f>(C98/B98)-1</f>
+        <f t="shared" si="12"/>
         <v>-0.10421263396502034</v>
       </c>
       <c r="D99" s="35">
-        <f>(D98/C98)-1</f>
+        <f t="shared" si="12"/>
         <v>0.30111417844522959</v>
       </c>
       <c r="E99" s="35">
-        <f>(E98/D98)-1</f>
+        <f t="shared" si="12"/>
         <v>2.0462721794058947E-2</v>
       </c>
       <c r="F99" s="35">
-        <f>(F98/E98)-1</f>
+        <f t="shared" si="12"/>
         <v>-3.9254823685961449E-2</v>
       </c>
       <c r="G99" s="35">
-        <f>(G98/F98)-1</f>
+        <f t="shared" si="12"/>
         <v>-0.491516620498615</v>
       </c>
       <c r="H99" s="35">
-        <f>(H98/G98)-1</f>
+        <f t="shared" si="12"/>
         <v>1.3844058563159685</v>
       </c>
       <c r="I99" s="35">
-        <f>(I98/H98)-1</f>
+        <f t="shared" si="12"/>
         <v>-6.2973011566471504E-2</v>
       </c>
       <c r="J99" s="35">
-        <f>(J98/I98)-1</f>
+        <f t="shared" si="12"/>
         <v>0.4372142639439196</v>
       </c>
       <c r="K99" s="35">
-        <f>(K98/J98)-1</f>
+        <f t="shared" si="12"/>
         <v>0.35605980277807237</v>
       </c>
       <c r="L99" s="35">
-        <f>(L98/K98)-1</f>
+        <f t="shared" si="12"/>
         <v>-1.3292673391195331E-3</v>
       </c>
       <c r="M99" s="35">
-        <f>(M98/L98)-1</f>
+        <f t="shared" si="12"/>
         <v>0.31459442530535542</v>
       </c>
-      <c r="N99" s="47">
-        <f>(N98/M98)-1</f>
+      <c r="N99" s="46">
+        <f t="shared" si="12"/>
         <v>0.3097081596188207</v>
       </c>
-      <c r="O99" s="40">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="P99" s="40">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="Q99" s="41">
+      <c r="O99" s="39">
+        <v>0.18</v>
+      </c>
+      <c r="P99" s="39">
+        <v>0.18</v>
+      </c>
+      <c r="Q99" s="40">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="R99" s="30">
-        <f>(N99+M99+L99+K99+J99)/5</f>
-        <v>0.28324947686140972</v>
+        <f>(N99+M99+L99+K99+J99+I99+H99+G99+F99+E99)/10</f>
+        <v>0.2227371506666028</v>
       </c>
     </row>
     <row r="100" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="O100" s="1">
         <f>O98/(1+$S$54)^O97</f>
-        <v>26520895585.568089</v>
+        <v>24448950617.94558</v>
       </c>
       <c r="P100" s="1">
         <f>P98/(1+$S$54)^P97</f>
-        <v>31985352553.915638</v>
+        <v>27182864316.450279</v>
       </c>
       <c r="Q100" s="1">
         <f>Q98/(1+$S$54)^Q97</f>
-        <v>902629944144.17114</v>
+        <v>767103231339.32117</v>
       </c>
     </row>
     <row r="102" spans="1:18" x14ac:dyDescent="0.2">
       <c r="N102" s="14" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="O102" s="14">
         <f>SUM(O100:Q100)</f>
-        <v>961136192283.65491</v>
+        <v>818735046273.71704</v>
       </c>
     </row>
     <row r="103" spans="1:18" x14ac:dyDescent="0.2">
       <c r="N103" s="14" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="O103" s="14">
         <f>S49</f>
@@ -5739,64 +5739,64 @@
       </c>
     </row>
     <row r="104" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="N104" s="53" t="s">
-        <v>125</v>
-      </c>
-      <c r="O104" s="53">
+      <c r="N104" s="52" t="s">
+        <v>123</v>
+      </c>
+      <c r="O104" s="52">
         <f>N35</f>
         <v>9830000000</v>
       </c>
     </row>
     <row r="105" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="N105" s="54" t="s">
+      <c r="N105" s="53" t="s">
+        <v>125</v>
+      </c>
+      <c r="O105" s="53">
+        <f>O102-O103+O104</f>
+        <v>751881046273.71704</v>
+      </c>
+    </row>
+    <row r="106" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="N106" s="52" t="s">
+        <v>126</v>
+      </c>
+      <c r="O106" s="52">
+        <v>1770000000</v>
+      </c>
+    </row>
+    <row r="107" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="N107" s="54" t="s">
         <v>127</v>
       </c>
-      <c r="O105" s="54">
-        <f>O102-O103+O104</f>
-        <v>894282192283.65491</v>
-      </c>
-    </row>
-    <row r="106" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="N106" s="53" t="s">
-        <v>128</v>
-      </c>
-      <c r="O106" s="53">
-        <v>1770000000</v>
-      </c>
-    </row>
-    <row r="107" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="N107" s="55" t="s">
-        <v>129</v>
-      </c>
-      <c r="O107" s="56">
+      <c r="O107" s="55">
         <f>O105/O106</f>
-        <v>505.24417643144346</v>
+        <v>424.79155156707179</v>
       </c>
     </row>
     <row r="108" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="N108" s="20" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="O108">
-        <v>147.07</v>
+        <v>149.82</v>
       </c>
     </row>
     <row r="110" spans="1:18" ht="17" x14ac:dyDescent="0.2">
-      <c r="N110" s="58" t="s">
-        <v>131</v>
-      </c>
-      <c r="O110" s="57" t="str">
+      <c r="N110" s="57" t="s">
+        <v>129</v>
+      </c>
+      <c r="O110" s="56" t="str">
         <f>IF(O107&gt;O108, "BUY", "SELL")</f>
         <v>BUY</v>
       </c>
     </row>
     <row r="111" spans="1:18" ht="17" x14ac:dyDescent="0.2">
-      <c r="N111" s="58" t="s">
-        <v>132</v>
-      </c>
-      <c r="O111" s="59">
+      <c r="N111" s="57" t="s">
+        <v>130</v>
+      </c>
+      <c r="O111" s="58">
         <f>(O107/O108)-1</f>
-        <v>2.4353993093863022</v>
+        <v>1.8353460924247216</v>
       </c>
     </row>
   </sheetData>

</xml_diff>